<commit_message>
fix download excel pinjam mr
</commit_message>
<xml_diff>
--- a/assets/upload/Laporan Peminjaman Rekam Medis - .xlsx
+++ b/assets/upload/Laporan Peminjaman Rekam Medis - .xlsx
@@ -137,10 +137,10 @@
     <t>test7</t>
   </si>
   <si>
+    <t>TR000008</t>
+  </si>
+  <si>
     <t>TR000007</t>
-  </si>
-  <si>
-    <t>TR000008</t>
   </si>
   <si>
     <t>testt</t>

</xml_diff>